<commit_message>
Upload: Final and stable autoomation setup
</commit_message>
<xml_diff>
--- a/Manual/Test-Case-Document/Test-Cases-Document.xlsx
+++ b/Manual/Test-Case-Document/Test-Cases-Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d09b73bd954f8bef/Desktop/Nopcommerce Project/Manual/Test-Case-Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:1_{1EFF21C9-A454-49D8-9CCC-2B6C184BE556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A96A1C-84A3-4059-809B-C53C86D6BC9A}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="13_ncr:1_{1EFF21C9-A454-49D8-9CCC-2B6C184BE556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16CCE44F-D265-4CF2-BF5D-7D4306E592C9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage_TC" sheetId="7" r:id="rId1"/>
@@ -465,27 +465,9 @@
     <t>Banner slides smoothly</t>
   </si>
   <si>
-    <t>Verify hero CTA visibility</t>
-  </si>
-  <si>
-    <t>Scroll to hero banner; Check CTA</t>
-  </si>
-  <si>
-    <t>CTA visible</t>
-  </si>
-  <si>
-    <t>Verify CTA redirection works</t>
-  </si>
-  <si>
-    <t>Click CTA; Validate redirect</t>
-  </si>
-  <si>
     <t>Redirects to correct page</t>
   </si>
   <si>
-    <t>Verify components after refresh</t>
-  </si>
-  <si>
     <t>Note components; Refresh; Compare</t>
   </si>
   <si>
@@ -1852,6 +1834,24 @@
   </si>
   <si>
     <t>Active item highlighted</t>
+  </si>
+  <si>
+    <t>Verify homepage featured products section is visible</t>
+  </si>
+  <si>
+    <t>Scroll to hero featured products section,check visibility</t>
+  </si>
+  <si>
+    <t>Featured products visible</t>
+  </si>
+  <si>
+    <t>Verify featured product redirection works</t>
+  </si>
+  <si>
+    <t>Click product; Validate redirect</t>
+  </si>
+  <si>
+    <t>Verify logo after refresh</t>
   </si>
 </sst>
 </file>
@@ -2241,15 +2241,15 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -2699,20 +2699,20 @@
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>146</v>
+      <c r="C16" t="s">
+        <v>603</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>147</v>
+        <v>604</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>148</v>
+        <v>605</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>10</v>
@@ -2729,19 +2729,19 @@
         <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>149</v>
+        <v>606</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>150</v>
+        <v>607</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>11</v>
@@ -2758,19 +2758,19 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>152</v>
+        <v>608</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>10</v>
@@ -2787,19 +2787,19 @@
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -2816,19 +2816,19 @@
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
@@ -2845,19 +2845,19 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>11</v>
@@ -2926,25 +2926,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -2955,25 +2955,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -2984,25 +2984,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -3013,25 +3013,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -3042,25 +3042,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -3071,25 +3071,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>10</v>
@@ -3100,25 +3100,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -3129,25 +3129,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>10</v>
@@ -3158,25 +3158,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -3187,25 +3187,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>10</v>
@@ -3216,25 +3216,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>10</v>
@@ -3245,25 +3245,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>27</v>
@@ -3274,25 +3274,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>27</v>
@@ -3303,25 +3303,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -3332,25 +3332,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>10</v>
@@ -3361,25 +3361,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>10</v>
@@ -3390,25 +3390,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>27</v>
@@ -3419,25 +3419,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -3448,25 +3448,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
@@ -3477,25 +3477,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
@@ -3563,25 +3563,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -3592,25 +3592,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -3621,25 +3621,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -3650,25 +3650,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -3679,25 +3679,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -3708,25 +3708,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>10</v>
@@ -3737,25 +3737,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>10</v>
@@ -3766,25 +3766,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>27</v>
@@ -3795,25 +3795,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -3824,25 +3824,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>10</v>
@@ -3853,25 +3853,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>10</v>
@@ -3882,25 +3882,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>27</v>
@@ -3911,25 +3911,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>10</v>
@@ -3940,25 +3940,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>10</v>
@@ -3969,25 +3969,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>11</v>
@@ -3998,25 +3998,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>10</v>
@@ -4027,25 +4027,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>10</v>
@@ -4056,25 +4056,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -4085,25 +4085,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
@@ -4114,25 +4114,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
@@ -4198,25 +4198,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -4227,25 +4227,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -4256,25 +4256,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -4285,25 +4285,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -4314,25 +4314,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -4343,25 +4343,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>11</v>
@@ -4372,25 +4372,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -4401,25 +4401,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>10</v>
@@ -4430,25 +4430,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>10</v>
@@ -4459,25 +4459,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>10</v>
@@ -4488,25 +4488,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>11</v>
@@ -4517,25 +4517,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>10</v>
@@ -4546,25 +4546,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>10</v>
@@ -4575,25 +4575,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -4604,25 +4604,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>27</v>
@@ -4633,25 +4633,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>27</v>
@@ -4662,25 +4662,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>11</v>
@@ -4691,25 +4691,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -4720,25 +4720,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>10</v>
@@ -4749,25 +4749,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
@@ -4835,25 +4835,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -4864,25 +4864,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -4893,25 +4893,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -4922,25 +4922,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -4951,25 +4951,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -4980,25 +4980,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>10</v>
@@ -5009,25 +5009,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -5038,25 +5038,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>11</v>
@@ -5067,25 +5067,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -5096,25 +5096,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>10</v>
@@ -5125,25 +5125,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>10</v>
@@ -5154,25 +5154,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>10</v>
@@ -5183,25 +5183,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>10</v>
@@ -5212,25 +5212,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>10</v>
@@ -5241,25 +5241,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>11</v>
@@ -5270,25 +5270,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>506</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>10</v>
@@ -5299,25 +5299,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>10</v>
@@ -5328,25 +5328,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -5357,25 +5357,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>10</v>
@@ -5386,25 +5386,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
@@ -5425,7 +5425,7 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -5472,25 +5472,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -5501,25 +5501,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -5530,25 +5530,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -5559,25 +5559,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -5588,25 +5588,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -5617,25 +5617,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>549</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>10</v>
@@ -5646,25 +5646,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -5675,25 +5675,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>10</v>
@@ -5704,25 +5704,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>27</v>
@@ -5733,25 +5733,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
@@ -5762,25 +5762,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>11</v>
@@ -5791,25 +5791,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>10</v>
@@ -5820,25 +5820,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
@@ -5849,25 +5849,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>10</v>
@@ -5878,25 +5878,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>11</v>
@@ -5907,25 +5907,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>10</v>
@@ -5936,25 +5936,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>10</v>
@@ -5965,25 +5965,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>599</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -5994,22 +5994,22 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>109</v>
@@ -6023,25 +6023,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>608</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>27</v>

</xml_diff>